<commit_message>
última actualización, cronogama-plan de gestion
</commit_message>
<xml_diff>
--- a/Desarrollo/SCPM/Gestión/SCPM_C.xlsx
+++ b/Desarrollo/SCPM/Gestión/SCPM_C.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miE1mOlOCrDkU2Ba3uZxc7KGxxCQg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgSvTQZhQjy0YLj/omPk66g0p32pg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Enfoque de desarrollo: </t>
   </si>
   <si>
-    <t>SCRUM</t>
+    <t>Clasico</t>
   </si>
   <si>
     <t>Inicio:</t>
@@ -78,13 +78,13 @@
     <t>Gestión y Negocio</t>
   </si>
   <si>
-    <t>Elaboracion del Plan del Proyecto</t>
-  </si>
-  <si>
-    <t>Plan del Proyecto</t>
-  </si>
-  <si>
-    <t>SCPM_PP</t>
+    <t>Elaboracion del Modelo Lean Canvas</t>
+  </si>
+  <si>
+    <t>Modelo Lean Canvas</t>
+  </si>
+  <si>
+    <t>SCPM_MLC.pdf</t>
   </si>
   <si>
     <t>Prado/GGC</t>
@@ -96,19 +96,19 @@
     <t xml:space="preserve">Cronograma </t>
   </si>
   <si>
-    <t>SCPM_C</t>
+    <t>SCPM_C.xlsx</t>
   </si>
   <si>
     <t>Quispe/GGC</t>
   </si>
   <si>
-    <t xml:space="preserve">Elaboracion del Plan CSM </t>
-  </si>
-  <si>
-    <t>Plan SCM</t>
-  </si>
-  <si>
-    <t>SCPM_PCSM</t>
+    <t>Elaboracion del Project Charter</t>
+  </si>
+  <si>
+    <t>Project Charter</t>
+  </si>
+  <si>
+    <t>SCPM_PC.docx</t>
   </si>
   <si>
     <t>Hito 1</t>
@@ -123,7 +123,7 @@
     <t>Documento de Requisitos</t>
   </si>
   <si>
-    <t>SCPM_DR</t>
+    <t>SCPM_DR.docx</t>
   </si>
   <si>
     <t>Sambrano/GGC</t>
@@ -135,7 +135,7 @@
     <t>Documento  de especificación de Requisitos</t>
   </si>
   <si>
-    <t>SCPM_DER</t>
+    <t>SCPM_DER.xlsx</t>
   </si>
   <si>
     <t>Elaboración de Diagrama de clase y entidad relacion</t>
@@ -144,7 +144,7 @@
     <t>Documento de diagrama y ER</t>
   </si>
   <si>
-    <t>SCPM_DDER</t>
+    <t>SCPM_DDER.pdf</t>
   </si>
   <si>
     <t>Elaboración de modelamiento de procesos</t>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">Diagrama de Procesos </t>
   </si>
   <si>
-    <t>SCPM_MP</t>
+    <t>SCPM_MP.pdf</t>
   </si>
   <si>
     <t>Diseño de la arquitectura de software</t>
@@ -162,7 +162,7 @@
     <t>Documento de arquitectura de software</t>
   </si>
   <si>
-    <t>SCPM_DAS</t>
+    <t>SCPM_DAS.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Diseño (prototipo) de la interfaz del producto software </t>
@@ -171,7 +171,7 @@
     <t>Documento de interfaces del producto</t>
   </si>
   <si>
-    <t>SCPM_DIP</t>
+    <t>SCPM_DIP.pdf</t>
   </si>
   <si>
     <t>Hito 2</t>
@@ -186,7 +186,7 @@
     <t>Base de Datos</t>
   </si>
   <si>
-    <t>SCPM_BD</t>
+    <t>SCPM_BD.docx</t>
   </si>
   <si>
     <t>Prado-Sambrano/GGC</t>
@@ -198,9 +198,6 @@
     <t>Tablas de la BD</t>
   </si>
   <si>
-    <t>SCPM_TBD</t>
-  </si>
-  <si>
     <t>Quispe-Prado/GGC</t>
   </si>
   <si>
@@ -210,19 +207,43 @@
     <t>Pagina Principal</t>
   </si>
   <si>
+    <t>Elaboración del login</t>
+  </si>
+  <si>
+    <t>Login de la Pagina Principal</t>
+  </si>
+  <si>
+    <t>Quispe-Prado-Sambrano/GGC</t>
+  </si>
+  <si>
     <t>Elaboración del Registro de Usuarios</t>
   </si>
   <si>
     <t>Registro de Usuarios</t>
   </si>
   <si>
-    <t>Elaboración del login</t>
-  </si>
-  <si>
-    <t>Login de la Pagina Principal</t>
-  </si>
-  <si>
-    <t>Quispe-Prado-Sambrano/GGC</t>
+    <t>Elaboración de interfaz de medicamentos</t>
+  </si>
+  <si>
+    <t>Mostrar medicamentos</t>
+  </si>
+  <si>
+    <t>Elaboración de la pagina de noticias</t>
+  </si>
+  <si>
+    <t>Noticias</t>
+  </si>
+  <si>
+    <t>Modulo de Comentarios</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Elaboración de editar cuenta</t>
+  </si>
+  <si>
+    <t>Editar Cuentas</t>
   </si>
   <si>
     <t>Hito 3</t>
@@ -231,19 +252,16 @@
     <t>Prueba / Despliegue</t>
   </si>
   <si>
-    <t>Elaboración de editar cuenta</t>
-  </si>
-  <si>
-    <t>Editar Cuentas</t>
-  </si>
-  <si>
-    <t>Elaboración de interfaz de medicamentos</t>
-  </si>
-  <si>
-    <t>Mostrar medicamentos</t>
-  </si>
-  <si>
-    <t>Documento de pruebas</t>
+    <t>Diagrama de secuencia, flujo de procesos</t>
+  </si>
+  <si>
+    <t>Documento de secuencias</t>
+  </si>
+  <si>
+    <t>SCPM_DS</t>
+  </si>
+  <si>
+    <t>Documento de casos de prueba</t>
   </si>
   <si>
     <t>Documentar pruebas integración/aceptación</t>
@@ -272,7 +290,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -309,7 +327,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FFFF0000"/>
@@ -317,10 +334,7 @@
     </font>
     <font>
       <color rgb="FFFF0000"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -329,27 +343,17 @@
     </font>
     <font>
       <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
     </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
-    <font>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -444,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -484,97 +488,91 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="13" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="17" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -794,12 +792,14 @@
     <col customWidth="1" min="1" max="1" width="12.88"/>
     <col customWidth="1" min="2" max="2" width="44.25"/>
     <col customWidth="1" min="3" max="3" width="35.0"/>
-    <col customWidth="1" min="4" max="4" width="11.88"/>
+    <col customWidth="1" min="4" max="4" width="14.38"/>
     <col customWidth="1" min="5" max="5" width="18.5"/>
     <col customWidth="1" min="6" max="6" width="12.75"/>
     <col customWidth="1" min="7" max="7" width="10.75"/>
     <col customWidth="1" min="8" max="8" width="11.38"/>
-    <col customWidth="1" min="9" max="26" width="9.38"/>
+    <col customWidth="1" min="9" max="9" width="9.38"/>
+    <col customWidth="1" min="10" max="10" width="17.38"/>
+    <col customWidth="1" min="11" max="26" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -855,7 +855,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="5">
-        <v>44469.0</v>
+        <v>44421.0</v>
       </c>
     </row>
     <row r="8">
@@ -912,7 +912,7 @@
         <v>44358.0</v>
       </c>
       <c r="H10" s="12">
-        <v>0.7</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -935,7 +935,7 @@
         <v>44363.0</v>
       </c>
       <c r="H11" s="12">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -958,7 +958,7 @@
         <v>44372.0</v>
       </c>
       <c r="H12" s="16">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
@@ -999,17 +999,17 @@
       <c r="D15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="14">
         <v>44372.0</v>
       </c>
       <c r="G15" s="14">
         <v>44377.0</v>
       </c>
-      <c r="H15" s="25">
-        <v>0.5</v>
+      <c r="H15" s="12">
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -1025,14 +1025,14 @@
       <c r="E16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="23">
         <v>44379.0</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="23">
         <v>44383.0</v>
       </c>
-      <c r="H16" s="27">
-        <v>0.5</v>
+      <c r="H16" s="24">
+        <v>1.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -1042,16 +1042,16 @@
       <c r="C17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="26">
         <v>44379.0</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="26">
         <v>44383.0</v>
       </c>
       <c r="H17" s="12">
@@ -1065,19 +1065,19 @@
       <c r="C18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="27">
         <v>44386.0</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="26">
         <v>44385.0</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="12">
         <v>1.0</v>
       </c>
     </row>
@@ -1088,19 +1088,19 @@
       <c r="C19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="26">
         <v>44379.0</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="26">
         <v>44384.0</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="12">
         <v>1.0</v>
       </c>
     </row>
@@ -1112,20 +1112,20 @@
       <c r="C20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="26">
         <v>44381.0</v>
       </c>
-      <c r="G20" s="32">
-        <v>44386.0</v>
-      </c>
-      <c r="H20" s="25">
-        <v>0.5</v>
+      <c r="G20" s="28">
+        <v>44391.0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -1138,24 +1138,24 @@
       <c r="F21" s="18">
         <v>44372.0</v>
       </c>
-      <c r="G21" s="33">
-        <v>44386.0</v>
+      <c r="G21" s="29">
+        <v>44393.0</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="31" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="10" t="s">
@@ -1169,85 +1169,83 @@
       <c r="C23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="10" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="31">
-        <v>44386.0</v>
-      </c>
-      <c r="G23" s="31">
-        <v>44393.0</v>
+      <c r="F23" s="26">
+        <v>44397.0</v>
+      </c>
+      <c r="G23" s="26">
+        <v>44400.0</v>
       </c>
       <c r="H23" s="12">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="13" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="10"/>
+      <c r="E24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="26">
+        <v>44397.0</v>
+      </c>
+      <c r="G24" s="26">
+        <v>44400.0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="B25" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="31">
-        <v>44386.0</v>
-      </c>
-      <c r="G24" s="31">
-        <v>44393.0</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="23" t="s">
+      <c r="C25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="26">
+        <v>44400.0</v>
+      </c>
+      <c r="G25" s="26">
+        <v>44407.0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="B26" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="31">
-        <v>44393.0</v>
-      </c>
-      <c r="G25" s="31">
-        <v>44400.0</v>
-      </c>
-      <c r="H25" s="25">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="37" t="s">
+      <c r="C26" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="31">
-        <v>44400.0</v>
-      </c>
-      <c r="G26" s="31">
+      <c r="F26" s="26">
+        <v>44398.0</v>
+      </c>
+      <c r="G26" s="26">
         <v>44407.0</v>
       </c>
-      <c r="H26" s="25">
-        <v>0.0</v>
+      <c r="H26" s="12">
+        <v>1.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -1259,268 +1257,271 @@
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="26">
+        <v>44400.0</v>
+      </c>
+      <c r="G27" s="26">
+        <v>44407.0</v>
+      </c>
+      <c r="H27" s="32">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="B28" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="29">
-        <v>44400.0</v>
-      </c>
-      <c r="G27" s="29">
-        <v>44407.0</v>
-      </c>
-      <c r="H27" s="12">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="38" t="s">
+      <c r="C28" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="39">
-        <v>44386.0</v>
-      </c>
-      <c r="G28" s="33">
-        <v>44400.0</v>
-      </c>
-      <c r="H28" s="40"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="26">
+        <v>44431.0</v>
+      </c>
+      <c r="G28" s="34">
+        <v>44414.0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="21"/>
+      <c r="C29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="26">
+        <v>44414.0</v>
+      </c>
+      <c r="G29" s="34">
+        <v>44421.0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="29">
-        <v>44407.0</v>
-      </c>
-      <c r="G30" s="41">
-        <v>44414.0</v>
+        <v>57</v>
+      </c>
+      <c r="F30" s="26">
+        <v>44421.0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>44428.0</v>
       </c>
       <c r="H30" s="12">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="31">
-        <v>44383.0</v>
-      </c>
-      <c r="G31" s="43">
+      <c r="C31" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="26">
+        <v>44428.0</v>
+      </c>
+      <c r="G31" s="37">
+        <v>44435.0</v>
+      </c>
+      <c r="H31" s="38">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="B32" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="40">
+        <v>44393.0</v>
+      </c>
+      <c r="G32" s="29">
+        <v>44435.0</v>
+      </c>
+      <c r="H32" s="41"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="B33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="B34" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="26">
+        <v>44435.0</v>
+      </c>
+      <c r="G34" s="35">
+        <v>44442.0</v>
+      </c>
+      <c r="H34" s="42">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="B35" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="26">
+        <v>44435.0</v>
+      </c>
+      <c r="G35" s="35">
+        <v>44442.0</v>
+      </c>
+      <c r="H35" s="42">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="B36" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="26">
+        <v>44435.0</v>
+      </c>
+      <c r="G36" s="35">
+        <v>44442.0</v>
+      </c>
+      <c r="H36" s="42">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="43">
         <v>44421.0</v>
       </c>
-      <c r="H31" s="25">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="31">
-        <v>44383.0</v>
-      </c>
-      <c r="G32" s="43">
-        <v>44421.0</v>
-      </c>
-      <c r="H32" s="44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="31">
-        <v>44383.0</v>
-      </c>
-      <c r="G33" s="43">
-        <v>44421.0</v>
-      </c>
-      <c r="H33" s="44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="45">
-        <v>44400.0</v>
-      </c>
-      <c r="G34" s="46">
-        <v>44421.0</v>
-      </c>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="H35" s="47"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
+      <c r="G37" s="29">
+        <v>44442.0</v>
+      </c>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-    </row>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2461,10 +2462,6 @@
     <row r="986" ht="15.75" customHeight="1"/>
     <row r="987" ht="15.75" customHeight="1"/>
     <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>

</xml_diff>